<commit_message>
Userstories planned last Sprint in 2017
</commit_message>
<xml_diff>
--- a/planning/User Story Version 2017 Start.xlsx
+++ b/planning/User Story Version 2017 Start.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="114">
   <si>
     <t>Geschwindigkeit</t>
   </si>
@@ -438,9 +438,6 @@
     <t>New Game (Tutto)</t>
   </si>
   <si>
-    <t>Pictures</t>
-  </si>
-  <si>
     <t>Export/Import intern MySQL Server</t>
   </si>
   <si>
@@ -457,13 +454,28 @@
   </si>
   <si>
     <t>Support</t>
+  </si>
+  <si>
+    <t>CSV import / export</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User </t>
+  </si>
+  <si>
+    <t>Statistik</t>
+  </si>
+  <si>
+    <t>Pictures (import)</t>
+  </si>
+  <si>
+    <t>DB Export import</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,12 +488,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -519,6 +525,27 @@
       <name val="Wingdings 2"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -684,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -707,109 +734,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1097,547 +1147,612 @@
   </sheetPr>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5546875" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="128.21875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5546875" style="38" customWidth="1"/>
+    <col min="5" max="5" width="4" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="128.21875" style="51" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="38"/>
+    <col min="11" max="11" width="22.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="28" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="11">
+      <c r="B2" s="31"/>
+      <c r="C2" s="32">
         <v>1</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="33">
         <f>IF(E2="","",MAX(D$1:D1)+1)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="34">
         <v>1</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="1"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="11">
+      <c r="B3" s="40"/>
+      <c r="C3" s="32">
         <f>MAX(C$2:C2)+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="33">
         <f>IF(E3="","",MAX(D$1:D2)+1)</f>
         <v>2</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="41">
         <v>1</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="1"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="11">
+      <c r="B4" s="40"/>
+      <c r="C4" s="32">
         <f>MAX(C$2:C3)+1</f>
         <v>3</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="33">
         <f>IF(E4="","",MAX(D$1:D3)+1)</f>
         <v>3</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="41">
         <v>1</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="1"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="11">
+      <c r="B5" s="40"/>
+      <c r="C5" s="32">
         <f>MAX(C$2:C4)+1</f>
         <v>4</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="33">
         <f>IF(E5="","",MAX(D$1:D4)+1)</f>
         <v>4</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="41">
         <v>4</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="37"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="11">
+      <c r="B6" s="44"/>
+      <c r="C6" s="32">
         <f>MAX(C$2:C5)+1</f>
         <v>5</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="33">
         <f>IF(E6="","",MAX(D$1:D5)+1)</f>
         <v>5</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="41">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="1"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11">
+      <c r="B7" s="40"/>
+      <c r="C7" s="32">
         <f>MAX(C$2:C6)+1</f>
         <v>6</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="33">
         <f>IF(E7="","",MAX(D$1:D6)+1)</f>
         <v>6</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="41">
         <v>4</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="1"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="11">
+      <c r="B8" s="44"/>
+      <c r="C8" s="32">
         <f>MAX(C$2:C7)+1</f>
         <v>7</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="33">
         <f>IF(E8="","",MAX(D$1:D7)+1)</f>
         <v>7</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="41">
         <v>5</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="1"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="37"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="22">
+      <c r="A9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33">
         <f>IF(E9="","",MAX(D$1:D8)+1)</f>
         <v>8</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="41">
         <v>5</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="1"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D10" s="22">
+      <c r="D10" s="33">
         <f>IF(E10="","",MAX(D$1:D9)+1)</f>
         <v>9</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="1"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D11" s="22">
+      <c r="D11" s="33">
         <f>IF(E11="","",MAX(D$1:D10)+1)</f>
         <v>10</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="41">
         <v>5</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="1"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D12" s="22">
+      <c r="D12" s="33">
         <f>IF(E12="","",MAX(D$1:D11)+1)</f>
         <v>11</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="41">
         <v>6</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="1"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D13" s="22">
+      <c r="D13" s="33">
         <f>IF(E13="","",MAX(D$1:D12)+1)</f>
         <v>12</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="41">
         <v>6</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="1"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="37"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D14" s="22">
+      <c r="D14" s="33">
         <f>IF(E14="","",MAX(D$1:D13)+1)</f>
         <v>13</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="41">
         <v>6</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="1"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D15" s="22">
+      <c r="D15" s="33">
         <f>IF(E15="","",MAX(D$1:D14)+1)</f>
         <v>14</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="41">
         <v>1</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" s="1"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D16" s="22">
+      <c r="D16" s="33">
         <f>IF(E16="","",MAX(D$1:D15)+1)</f>
         <v>15</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="41">
         <v>7</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="1"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="37"/>
     </row>
     <row r="17" spans="4:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="22">
+      <c r="D17" s="33">
         <f>IF(E17="","",MAX(D$1:D16)+1)</f>
         <v>16</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="41">
         <v>4</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1" t="s">
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D18" s="22">
+      <c r="D18" s="33">
         <f>IF(E18="","",MAX(D$1:D17)+1)</f>
         <v>17</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="33">
         <v>1</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="I18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="1"/>
+      <c r="G18" s="49"/>
+      <c r="I18" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="37"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D19" s="22">
+      <c r="D19" s="33">
         <f>IF(E19="","",MAX(D$1:D18)+1)</f>
         <v>18</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="50">
         <v>7</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="G19" s="38">
+        <v>1</v>
+      </c>
+      <c r="I19" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D20" s="22">
+      <c r="D20" s="33">
         <f>IF(E20="","",MAX(D$1:D19)+1)</f>
         <v>19</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="50">
         <v>1</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="G20" s="38">
+        <v>0</v>
+      </c>
+      <c r="I20" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D21" s="22">
+      <c r="D21" s="33">
         <f>IF(E21="","",MAX(D$1:D20)+1)</f>
         <v>20</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="50">
         <v>1</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="F21" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D22" s="22">
+      <c r="D22" s="33">
         <f>IF(E22="","",MAX(D$1:D21)+1)</f>
         <v>21</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="50">
         <v>1</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="48" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D23" s="22">
+      <c r="D23" s="33">
         <f>IF(E23="","",MAX(D$1:D22)+1)</f>
         <v>22</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="50">
         <v>1</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="G23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D24" s="22" t="str">
+      <c r="D24" s="33">
         <f>IF(E24="","",MAX(D$1:D23)+1)</f>
-        <v/>
+        <v>23</v>
+      </c>
+      <c r="E24" s="50">
+        <v>2</v>
+      </c>
+      <c r="F24" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="38">
+        <v>2</v>
+      </c>
+      <c r="I24" s="37" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D25" s="22" t="str">
+      <c r="D25" s="33">
         <f>IF(E25="","",MAX(D$1:D24)+1)</f>
-        <v/>
+        <v>24</v>
+      </c>
+      <c r="E25" s="50">
+        <v>3</v>
+      </c>
+      <c r="F25" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="38">
+        <v>1</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="33">
+        <f>IF(E26="","",MAX(D$1:D25)+1)</f>
+        <v>25</v>
+      </c>
+      <c r="E26" s="50">
+        <v>4</v>
+      </c>
+      <c r="F26" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="38">
+        <v>2</v>
+      </c>
+      <c r="I26" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="33">
+        <f>IF(E27="","",MAX(D$1:D26)+1)</f>
+        <v>26</v>
+      </c>
+      <c r="E27" s="50">
+        <v>4</v>
+      </c>
+      <c r="F27" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="38">
+        <v>3</v>
+      </c>
+      <c r="I27" s="37" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D30" s="1"/>
+      <c r="D30" s="37"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="26"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="26"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="26"/>
+      <c r="A36" s="54"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="53"/>
     </row>
     <row r="42" spans="1:3" ht="14.7" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" s="1"/>
+      <c r="D49" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1677,7 +1792,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1692,7 +1807,7 @@
       <c r="E1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="14" t="s">
         <v>62</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -1700,12 +1815,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="22">
+      <c r="A2" s="12">
         <f>IF(B2="","",MAX(A$1:A1)+1)</f>
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>100</v>
@@ -1718,7 +1833,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="22">
+      <c r="A3" s="12">
         <f>IF(B3="","",MAX(A$1:A2)+1)</f>
         <v>2</v>
       </c>
@@ -1733,7 +1848,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="12">
         <f>IF(B4="","",MAX(A$1:A3)+1)</f>
         <v>3</v>
       </c>
@@ -1751,7 +1866,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="A5" s="12">
         <f>IF(B5="","",MAX(A$1:A4)+1)</f>
         <v>4</v>
       </c>
@@ -1769,7 +1884,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
+      <c r="A6" s="12">
         <f>IF(B6="","",MAX(A$1:A5)+1)</f>
         <v>5</v>
       </c>
@@ -1787,7 +1902,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="12">
         <f>IF(B7="","",MAX(A$1:A6)+1)</f>
         <v>6</v>
       </c>
@@ -1805,7 +1920,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="12">
         <f>IF(B8="","",MAX(A$1:A7)+1)</f>
         <v>7</v>
       </c>
@@ -1823,7 +1938,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="12">
         <f>IF(B9="","",MAX(A$1:A8)+1)</f>
         <v>8</v>
       </c>
@@ -1841,7 +1956,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="A10" s="12">
         <f>IF(B10="","",MAX(A$1:A9)+1)</f>
         <v>9</v>
       </c>
@@ -1859,7 +1974,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="12">
         <f>IF(B11="","",MAX(A$1:A10)+1)</f>
         <v>10</v>
       </c>
@@ -1877,7 +1992,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+      <c r="A12" s="12">
         <f>IF(B12="","",MAX(A$1:A11)+1)</f>
         <v>11</v>
       </c>
@@ -1895,7 +2010,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="22">
+      <c r="A13" s="12">
         <f>IF(B13="","",MAX(A$1:A12)+1)</f>
         <v>12</v>
       </c>
@@ -1910,7 +2025,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="22">
+      <c r="A14" s="12">
         <f>IF(B14="","",MAX(A$1:A13)+1)</f>
         <v>13</v>
       </c>
@@ -1925,7 +2040,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="22">
+      <c r="A15" s="12">
         <f>IF(B15="","",MAX(A$1:A14)+1)</f>
         <v>14</v>
       </c>
@@ -1943,7 +2058,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="22">
+      <c r="A16" s="12">
         <f>IF(B16="","",MAX(A$1:A15)+1)</f>
         <v>15</v>
       </c>
@@ -1958,7 +2073,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="22">
+      <c r="A17" s="12">
         <f>IF(B17="","",MAX(A$1:A16)+1)</f>
         <v>16</v>
       </c>
@@ -1973,7 +2088,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="22">
+      <c r="A18" s="12">
         <f>IF(B18="","",MAX(A$1:A17)+1)</f>
         <v>17</v>
       </c>
@@ -1991,7 +2106,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="22">
+      <c r="A19" s="12">
         <f>IF(B19="","",MAX(A$1:A18)+1)</f>
         <v>18</v>
       </c>
@@ -2010,7 +2125,7 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="A20" s="12">
         <f>IF(B20="","",MAX(A$1:A19)+1)</f>
         <v>19</v>
       </c>
@@ -2026,7 +2141,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="22">
+      <c r="A21" s="12">
         <f>IF(B21="","",MAX(A$1:A20)+1)</f>
         <v>20</v>
       </c>
@@ -2042,7 +2157,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="22">
+      <c r="A22" s="12">
         <f>IF(B22="","",MAX(A$1:A21)+1)</f>
         <v>21</v>
       </c>
@@ -2061,12 +2176,12 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="22">
+      <c r="A23" s="12">
         <f>IF(B23="","",MAX(A$1:A22)+1)</f>
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>35</v>
@@ -2077,7 +2192,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="22">
+      <c r="A24" s="12">
         <f>IF(B24="","",MAX(A$1:A23)+1)</f>
         <v>23</v>
       </c>
@@ -2096,116 +2211,116 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="str">
+      <c r="A25" s="12" t="str">
         <f>IF(B25="","",MAX(A$1:A24)+1)</f>
         <v/>
       </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="str">
+      <c r="A26" s="12" t="str">
         <f>IF(B26="","",MAX(A$1:A25)+1)</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="str">
+      <c r="A27" s="12" t="str">
         <f>IF(B27="","",MAX(A$1:A26)+1)</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
+      <c r="A29" s="12"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
+      <c r="A30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
+      <c r="A31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
+      <c r="A32" s="12"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+      <c r="A33" s="12"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
+      <c r="A34" s="12"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
+      <c r="A35" s="12"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
+      <c r="A36" s="12"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
+      <c r="A37" s="12"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
+      <c r="A38" s="12"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="22"/>
+      <c r="A39" s="12"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
+      <c r="A40" s="12"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
+      <c r="A41" s="12"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
+      <c r="A42" s="12"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="22"/>
+      <c r="A43" s="12"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="22"/>
+      <c r="A44" s="12"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="22"/>
+      <c r="A45" s="12"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
+      <c r="A46" s="12"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
+      <c r="A47" s="12"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="22"/>
+      <c r="A48" s="12"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="22"/>
+      <c r="A49" s="12"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="22"/>
+      <c r="A50" s="12"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
+      <c r="A51" s="12"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
+      <c r="A52" s="12"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
+      <c r="A53" s="12"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
+      <c r="A54" s="12"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="22"/>
+      <c r="A55" s="12"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="22"/>
+      <c r="A56" s="12"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="22"/>
+      <c r="A57" s="12"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="22"/>
+      <c r="A58" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2236,37 +2351,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>105</v>
+      <c r="H1" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="22">
+      <c r="A2" s="12">
         <f>IF(B2="","",MAX(A$1:A1)+1)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2281,11 +2396,11 @@
         <v>88</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="22">
+      <c r="A3" s="12">
         <f>IF(B3="","",MAX(A$1:A2)+1)</f>
         <v>2</v>
       </c>
@@ -2304,11 +2419,11 @@
         <v>89</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="12">
         <f>IF(B4="","",MAX(A$1:A3)+1)</f>
         <v>3</v>
       </c>
@@ -2327,11 +2442,11 @@
         <v>90</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="A5" s="12">
         <f>IF(B5="","",MAX(A$1:A4)+1)</f>
         <v>4</v>
       </c>
@@ -2350,11 +2465,11 @@
         <v>89</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
+      <c r="A6" s="12">
         <f>IF(B6="","",MAX(A$1:A5)+1)</f>
         <v>5</v>
       </c>
@@ -2375,15 +2490,15 @@
         <v>87</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="12">
         <f>IF(B7="","",MAX(A$1:A6)+1)</f>
         <v>6</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2400,15 +2515,15 @@
         <v>92</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="12">
         <f>IF(B8="","",MAX(A$1:A7)+1)</f>
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -2423,15 +2538,15 @@
         <v>89</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="12">
         <f>IF(B9="","",MAX(A$1:A8)+1)</f>
         <v>8</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2446,14 +2561,14 @@
         <v>86</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="str">
+      <c r="A10" s="12" t="str">
         <f>IF(B10="","",MAX(A$1:A9)+1)</f>
         <v/>
       </c>
@@ -2464,7 +2579,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="str">
+      <c r="A11" s="12" t="str">
         <f>IF(B11="","",MAX(A$1:A10)+1)</f>
         <v/>
       </c>
@@ -2475,11 +2590,11 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="str">
+      <c r="A12" s="12" t="str">
         <f>IF(B12="","",MAX(A$1:A11)+1)</f>
         <v/>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2487,7 +2602,7 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="str">
+      <c r="A13" s="12" t="str">
         <f>IF(B13="","",MAX(A$1:A12)+1)</f>
         <v/>
       </c>
@@ -2527,7 +2642,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="21"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4"/>
       <c r="D17" s="10"/>
       <c r="E17" s="1"/>
@@ -2535,7 +2650,7 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="21"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2562,298 +2677,298 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="41" customWidth="1"/>
-    <col min="3" max="3" width="102.77734375" style="39" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.21875" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="39"/>
+    <col min="1" max="1" width="3.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="102.77734375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="22">
+      <c r="A2" s="12">
         <f>IF(B2="","",MAX(A$1:A1)+1)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="22">
+      <c r="A3" s="12">
         <f>IF(B3="","",MAX(A$1:A2)+1)</f>
         <v>2</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="12">
         <f>IF(B4="","",MAX(A$1:A3)+1)</f>
         <v>3</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="A5" s="12">
         <f>IF(B5="","",MAX(A$1:A4)+1)</f>
         <v>4</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40" t="s">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="40"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
+      <c r="A6" s="12">
         <f>IF(B6="","",MAX(A$1:A5)+1)</f>
         <v>5</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="12">
         <f>IF(B7="","",MAX(A$1:A6)+1)</f>
         <v>6</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40" t="s">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="12">
         <f>IF(B8="","",MAX(A$1:A7)+1)</f>
         <v>7</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="40"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="12">
         <f>IF(B9="","",MAX(A$1:A8)+1)</f>
         <v>8</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="40"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="A10" s="12">
         <f>IF(B10="","",MAX(A$1:A9)+1)</f>
         <v>9</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="40"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="12">
         <f>IF(B11="","",MAX(A$1:A10)+1)</f>
         <v>10</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="19" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="str">
+      <c r="A12" s="12" t="str">
         <f>IF(B12="","",MAX(A$1:A11)+1)</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="str">
+      <c r="A13" s="12" t="str">
         <f>IF(B13="","",MAX(A$1:A12)+1)</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="str">
+      <c r="A14" s="12" t="str">
         <f>IF(B14="","",MAX(A$1:A13)+1)</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="str">
+      <c r="A15" s="12" t="str">
         <f>IF(B15="","",MAX(A$1:A14)+1)</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="str">
+      <c r="A16" s="12" t="str">
         <f>IF(B16="","",MAX(A$1:A15)+1)</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="str">
+      <c r="A17" s="12" t="str">
         <f>IF(B17="","",MAX(A$1:A16)+1)</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="str">
+      <c r="A18" s="12" t="str">
         <f>IF(B18="","",MAX(A$1:A17)+1)</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="str">
+      <c r="A19" s="12" t="str">
         <f>IF(B19="","",MAX(A$1:A18)+1)</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
+      <c r="A22" s="19"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
+      <c r="A23" s="19"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
+      <c r="A24" s="19"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
+      <c r="A25" s="19"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
+      <c r="A26" s="19"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
+      <c r="A27" s="19"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
+      <c r="A28" s="19"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
+      <c r="A29" s="19"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
+      <c r="A30" s="19"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
+      <c r="A31" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactoring Teil 2 inkl. Dokumente integriert
</commit_message>
<xml_diff>
--- a/planning/User Story Version 2017 Start.xlsx
+++ b/planning/User Story Version 2017 Start.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WISS\git\Lernkartei2017\Lernkartei_2017\planning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DD35D8E1-3915-454D-9687-7D6A7352AE2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10200" windowHeight="4176"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="14244" windowHeight="6996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funktionen" sheetId="5" r:id="rId1"/>
-    <sheet name="Bedienfunktion" sheetId="2" r:id="rId2"/>
-    <sheet name="DB(F&amp;Q)" sheetId="7" r:id="rId3"/>
-    <sheet name="Qualität" sheetId="3" r:id="rId4"/>
+    <sheet name="Persistenz" sheetId="7" r:id="rId2"/>
+    <sheet name="Q" sheetId="3" r:id="rId3"/>
+    <sheet name="Usability" sheetId="2" r:id="rId4"/>
+    <sheet name="Errors" sheetId="8" r:id="rId5"/>
+    <sheet name="ToDo" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Design">#REF!</definedName>
     <definedName name="Funktionen">Funktionen!$1:$1048576</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
+  <oleSize ref="A3:H19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="144">
   <si>
     <t>Geschwindigkeit</t>
   </si>
@@ -470,12 +469,102 @@
   <si>
     <t>DB Export import</t>
   </si>
+  <si>
+    <t>Pts.</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>States:</t>
+  </si>
+  <si>
+    <t>PREP</t>
+  </si>
+  <si>
+    <t>WORK</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>READY</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>Nicht vollst. Geklärt</t>
+  </si>
+  <si>
+    <t>Bereit zum impl.</t>
+  </si>
+  <si>
+    <t>Am Umsetzen</t>
+  </si>
+  <si>
+    <t>Am Testen</t>
+  </si>
+  <si>
+    <t>Integriert</t>
+  </si>
+  <si>
+    <t>Depreciated</t>
+  </si>
+  <si>
+    <t>Kosmetik</t>
+  </si>
+  <si>
+    <t>Verbesserungsvorschläge</t>
+  </si>
+  <si>
+    <t>innere Qualität: Dinge richtig tun</t>
+  </si>
+  <si>
+    <t>äussere Qualität: das Richtige tun</t>
+  </si>
+  <si>
+    <t>Fehler darf Sprint nicht verlassen (Fehlerkategorie 2: mittel)</t>
+  </si>
+  <si>
+    <t>Betrifft Alle und sofort (Fehlerkategoie 1: schwerwiegend, alles steht)</t>
+  </si>
+  <si>
+    <t>technische Angelegenheiten</t>
+  </si>
+  <si>
+    <t>Fehlerkategorie 3: leicht</t>
+  </si>
+  <si>
+    <t>Werden auf GitHub verwaltet über Issues</t>
+  </si>
+  <si>
+    <t>Alle arbeiten sofort an der Lösung des Problems</t>
+  </si>
+  <si>
+    <t>Version 2017 startet nicht mehr</t>
+  </si>
+  <si>
+    <t>Werden als dringende Tasks für diesen Sprint im Sprintbacklog umgewandelt</t>
+  </si>
+  <si>
+    <t>Einträge in Issues verwaltet</t>
+  </si>
+  <si>
+    <t>Werden auf GitHub verwaltet über Issues (evtl. auf ToDo verweisen)</t>
+  </si>
+  <si>
+    <t>Werden auf GitHub verwaltet über Issues, werden als Issue erledigt oder evtl. als Task oder User Story eingeplant</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +636,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -598,7 +696,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -707,11 +805,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -772,12 +950,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -788,12 +960,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -825,14 +991,47 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -840,26 +1039,30 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,619 +1343,730 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.21875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5546875" style="38" customWidth="1"/>
-    <col min="5" max="5" width="4" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="128.21875" style="51" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="38"/>
-    <col min="11" max="11" width="22.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="38"/>
+    <col min="1" max="1" width="15.5546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5546875" style="34" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="4" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="128.21875" style="43" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="34"/>
+    <col min="13" max="13" width="22.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.5546875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="H1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="I1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="J1" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="K1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="L1" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32">
+      <c r="B2" s="52"/>
+      <c r="C2" s="28">
         <v>1</v>
       </c>
-      <c r="D2" s="33">
-        <f>IF(E2="","",MAX(D$1:D1)+1)</f>
+      <c r="D2" s="29">
+        <f>IF(G2="","",MAX(D$1:D1)+1)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30">
         <v>1</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="H2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="I2" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="37"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="J2" s="32"/>
+      <c r="K2" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="33"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="32">
+      <c r="B3" s="36"/>
+      <c r="C3" s="28">
         <f>MAX(C$2:C2)+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="33">
-        <f>IF(E3="","",MAX(D$1:D2)+1)</f>
+      <c r="D3" s="29">
+        <f>IF(G3="","",MAX(D$1:D2)+1)</f>
         <v>2</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="37">
         <v>1</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="H3" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="37"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="33"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="32">
+      <c r="B4" s="36"/>
+      <c r="C4" s="28">
         <f>MAX(C$2:C3)+1</f>
         <v>3</v>
       </c>
-      <c r="D4" s="33">
-        <f>IF(E4="","",MAX(D$1:D3)+1)</f>
+      <c r="D4" s="29">
+        <f>IF(G4="","",MAX(D$1:D3)+1)</f>
         <v>3</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="37">
         <v>1</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="H4" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="I4" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="37"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="J4" s="32"/>
+      <c r="K4" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="32">
+      <c r="B5" s="36"/>
+      <c r="C5" s="28">
         <f>MAX(C$2:C4)+1</f>
         <v>4</v>
       </c>
-      <c r="D5" s="33">
-        <f>IF(E5="","",MAX(D$1:D4)+1)</f>
+      <c r="D5" s="29">
+        <f>IF(G5="","",MAX(D$1:D4)+1)</f>
         <v>4</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="37">
         <v>4</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="H5" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="I5" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="37"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+      <c r="J5" s="32"/>
+      <c r="K5" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="32">
+      <c r="B6" s="50"/>
+      <c r="C6" s="28">
         <f>MAX(C$2:C5)+1</f>
         <v>5</v>
       </c>
-      <c r="D6" s="33">
-        <f>IF(E6="","",MAX(D$1:D5)+1)</f>
+      <c r="D6" s="29">
+        <f>IF(G6="","",MAX(D$1:D5)+1)</f>
         <v>5</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="37">
         <v>4</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="H6" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="I6" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="37"/>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="J6" s="33"/>
+      <c r="K6" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="32">
+      <c r="B7" s="36"/>
+      <c r="C7" s="28">
         <f>MAX(C$2:C6)+1</f>
         <v>6</v>
       </c>
-      <c r="D7" s="33">
-        <f>IF(E7="","",MAX(D$1:D6)+1)</f>
+      <c r="D7" s="29">
+        <f>IF(G7="","",MAX(D$1:D6)+1)</f>
         <v>6</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="37">
         <v>4</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="H7" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="37"/>
-    </row>
-    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="32">
+      <c r="B8" s="50"/>
+      <c r="C8" s="28">
         <f>MAX(C$2:C7)+1</f>
         <v>7</v>
       </c>
-      <c r="D8" s="33">
-        <f>IF(E8="","",MAX(D$1:D7)+1)</f>
+      <c r="D8" s="29">
+        <f>IF(G8="","",MAX(D$1:D7)+1)</f>
         <v>7</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="37">
         <v>5</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="H8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="I8" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="37"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33">
-        <f>IF(E9="","",MAX(D$1:D8)+1)</f>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29">
+        <f>IF(G9="","",MAX(D$1:D8)+1)</f>
         <v>8</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="37">
         <v>5</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="H9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="I9" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="37"/>
-    </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D10" s="33">
-        <f>IF(E10="","",MAX(D$1:D9)+1)</f>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" s="33"/>
+    </row>
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D10" s="29">
+        <f>IF(G10="","",MAX(D$1:D9)+1)</f>
         <v>9</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="37">
         <v>5</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="H10" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="I10" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="37"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D11" s="33">
-        <f>IF(E11="","",MAX(D$1:D10)+1)</f>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="33"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="29">
+        <f>IF(G11="","",MAX(D$1:D10)+1)</f>
         <v>10</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="37">
         <v>5</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="H11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="I11" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="37"/>
-    </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D12" s="33">
-        <f>IF(E12="","",MAX(D$1:D11)+1)</f>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="33"/>
+    </row>
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="A12" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="29">
+        <f>IF(G12="","",MAX(D$1:D11)+1)</f>
         <v>11</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="37">
         <v>6</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="H12" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="37"/>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D13" s="33">
-        <f>IF(E13="","",MAX(D$1:D12)+1)</f>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="33"/>
+    </row>
+    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="59"/>
+      <c r="D13" s="29">
+        <f>IF(G13="","",MAX(D$1:D12)+1)</f>
         <v>12</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="37">
         <v>6</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="H13" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="I13" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D14" s="33">
-        <f>IF(E14="","",MAX(D$1:D13)+1)</f>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="33"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="29">
+        <f>IF(G14="","",MAX(D$1:D13)+1)</f>
         <v>13</v>
       </c>
-      <c r="E14" s="41">
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="37">
         <v>6</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="H14" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="I14" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D15" s="33">
-        <f>IF(E15="","",MAX(D$1:D14)+1)</f>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="33"/>
+    </row>
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="29">
+        <f>IF(G15="","",MAX(D$1:D14)+1)</f>
         <v>14</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="37">
         <v>1</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="H15" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" s="37"/>
-    </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D16" s="33">
-        <f>IF(E16="","",MAX(D$1:D15)+1)</f>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" s="33"/>
+    </row>
+    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="59"/>
+      <c r="D16" s="29">
+        <f>IF(G16="","",MAX(D$1:D15)+1)</f>
         <v>15</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="37">
         <v>7</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="H16" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="I16" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="4:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="33">
-        <f>IF(E17="","",MAX(D$1:D16)+1)</f>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" s="33"/>
+    </row>
+    <row r="17" spans="1:14" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="59"/>
+      <c r="D17" s="29">
+        <f>IF(G17="","",MAX(D$1:D16)+1)</f>
         <v>16</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="37">
         <v>4</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="H17" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D18" s="33">
-        <f>IF(E18="","",MAX(D$1:D17)+1)</f>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="60"/>
+      <c r="D18" s="29">
+        <f>IF(G18="","",MAX(D$1:D17)+1)</f>
         <v>17</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29">
         <v>1</v>
       </c>
-      <c r="F18" s="49" t="s">
+      <c r="H18" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="49"/>
-      <c r="I18" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="37"/>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D19" s="33">
-        <f>IF(E19="","",MAX(D$1:D18)+1)</f>
+      <c r="I18" s="41"/>
+      <c r="K18" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D19" s="29">
+        <f>IF(G19="","",MAX(D$1:D18)+1)</f>
         <v>18</v>
       </c>
-      <c r="E19" s="50">
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="42">
         <v>7</v>
       </c>
-      <c r="F19" s="51" t="s">
+      <c r="H19" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="38">
+      <c r="I19" s="34">
         <v>1</v>
       </c>
-      <c r="I19" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D20" s="33">
-        <f>IF(E20="","",MAX(D$1:D19)+1)</f>
+      <c r="K19" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D20" s="29">
+        <f>IF(G20="","",MAX(D$1:D19)+1)</f>
         <v>19</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="42">
         <v>1</v>
       </c>
-      <c r="F20" s="51" t="s">
+      <c r="H20" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="38">
+      <c r="I20" s="34">
         <v>0</v>
       </c>
-      <c r="I20" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D21" s="33">
-        <f>IF(E21="","",MAX(D$1:D20)+1)</f>
+      <c r="K20" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D21" s="29">
+        <f>IF(G21="","",MAX(D$1:D20)+1)</f>
         <v>20</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="42">
         <v>1</v>
       </c>
-      <c r="F21" s="51" t="s">
+      <c r="H21" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="I21" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D22" s="33">
-        <f>IF(E22="","",MAX(D$1:D21)+1)</f>
+      <c r="K21" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D22" s="29">
+        <f>IF(G22="","",MAX(D$1:D21)+1)</f>
         <v>21</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="42">
         <v>1</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="H22" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D23" s="33">
-        <f>IF(E23="","",MAX(D$1:D22)+1)</f>
+      <c r="K22" s="40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D23" s="29">
+        <f>IF(G23="","",MAX(D$1:D22)+1)</f>
         <v>22</v>
       </c>
-      <c r="E23" s="50">
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="42">
         <v>1</v>
       </c>
-      <c r="F23" s="51" t="s">
+      <c r="H23" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D24" s="33">
-        <f>IF(E24="","",MAX(D$1:D23)+1)</f>
+      <c r="K23" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D24" s="29">
+        <f>IF(G24="","",MAX(D$1:D23)+1)</f>
         <v>23</v>
       </c>
-      <c r="E24" s="50">
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="42">
         <v>2</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="H24" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="G24" s="38">
+      <c r="I24" s="34">
         <v>2</v>
       </c>
-      <c r="I24" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D25" s="33">
-        <f>IF(E25="","",MAX(D$1:D24)+1)</f>
+      <c r="K24" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D25" s="29">
+        <f>IF(G25="","",MAX(D$1:D24)+1)</f>
         <v>24</v>
       </c>
-      <c r="E25" s="50">
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="42">
         <v>3</v>
       </c>
-      <c r="F25" s="51" t="s">
+      <c r="H25" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="G25" s="38">
+      <c r="I25" s="34">
         <v>1</v>
       </c>
-      <c r="I25" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D26" s="33">
-        <f>IF(E26="","",MAX(D$1:D25)+1)</f>
+      <c r="K25" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D26" s="29">
+        <f>IF(G26="","",MAX(D$1:D25)+1)</f>
         <v>25</v>
       </c>
-      <c r="E26" s="50">
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="42">
         <v>4</v>
       </c>
-      <c r="F26" s="51" t="s">
+      <c r="H26" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="G26" s="38">
+      <c r="I26" s="34">
         <v>2</v>
       </c>
-      <c r="I26" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D27" s="33">
-        <f>IF(E27="","",MAX(D$1:D26)+1)</f>
+      <c r="K26" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D27" s="29">
+        <f>IF(G27="","",MAX(D$1:D26)+1)</f>
         <v>26</v>
       </c>
-      <c r="E27" s="50">
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="42">
         <v>4</v>
       </c>
-      <c r="F27" s="51" t="s">
+      <c r="H27" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="G27" s="38">
+      <c r="I27" s="34">
         <v>3</v>
       </c>
-      <c r="I27" s="37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D30" s="37"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="53"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="52"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="53"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="54"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="53"/>
-    </row>
-    <row r="42" spans="1:3" ht="14.7" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" s="37"/>
+      <c r="K27" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="46"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="44"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="46"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="44"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="45"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="44"/>
+    </row>
+    <row r="42" spans="1:14" ht="14.7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1770,14 +2084,763 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <f>IF(D2="","",MAX(A$1:A1)+1)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <f>IF(D3="","",MAX(A$1:A2)+1)</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <f>IF(D4="","",MAX(A$1:A3)+1)</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <f>IF(D5="","",MAX(A$1:A4)+1)</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <f>IF(D6="","",MAX(A$1:A5)+1)</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <f>IF(D7="","",MAX(A$1:A6)+1)</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <f>IF(D8="","",MAX(A$1:A7)+1)</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <f>IF(D9="","",MAX(A$1:A8)+1)</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="str">
+        <f>IF(D10="","",MAX(A$1:A9)+1)</f>
+        <v/>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="str">
+        <f>IF(D11="","",MAX(A$1:A10)+1)</f>
+        <v/>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="str">
+        <f>IF(D12="","",MAX(A$1:A11)+1)</f>
+        <v/>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="str">
+        <f>IF(D13="","",MAX(A$1:A12)+1)</f>
+        <v/>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D18" s="11"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="102.77734375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5546875" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <f>IF(D2="","",MAX(A$1:A1)+1)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <f>IF(D3="","",MAX(A$1:A2)+1)</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <f>IF(D4="","",MAX(A$1:A3)+1)</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <f>IF(D5="","",MAX(A$1:A4)+1)</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <f>IF(D6="","",MAX(A$1:A5)+1)</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <f>IF(D7="","",MAX(A$1:A6)+1)</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <f>IF(D8="","",MAX(A$1:A7)+1)</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <f>IF(D9="","",MAX(A$1:A8)+1)</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <f>IF(D10="","",MAX(A$1:A9)+1)</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <f>IF(D11="","",MAX(A$1:A10)+1)</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="str">
+        <f>IF(D12="","",MAX(A$1:A11)+1)</f>
+        <v/>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="str">
+        <f>IF(D13="","",MAX(A$1:A12)+1)</f>
+        <v/>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="str">
+        <f>IF(D17="","",MAX(A$1:A16)+1)</f>
+        <v/>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="str">
+        <f>IF(D18="","",MAX(A$1:A17)+1)</f>
+        <v/>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="str">
+        <f>IF(D19="","",MAX(A$1:A18)+1)</f>
+        <v/>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:F12"/>
     </sheetView>
   </sheetViews>
@@ -2328,650 +3391,101 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F05CC9-D724-4956-A465-5DEFDDE9DF91}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
-    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="102.77734375" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
-        <f>IF(B2="","",MAX(A$1:A1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
-        <f>IF(B3="","",MAX(A$1:A2)+1)</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <f>IF(B4="","",MAX(A$1:A3)+1)</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
-        <f>IF(B5="","",MAX(A$1:A4)+1)</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
-        <f>IF(B6="","",MAX(A$1:A5)+1)</f>
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <f>IF(B7="","",MAX(A$1:A6)+1)</f>
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
-        <f>IF(B8="","",MAX(A$1:A7)+1)</f>
-        <v>7</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
-        <f>IF(B9="","",MAX(A$1:A8)+1)</f>
-        <v>8</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="str">
-        <f>IF(B10="","",MAX(A$1:A9)+1)</f>
-        <v/>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="str">
-        <f>IF(B11="","",MAX(A$1:A10)+1)</f>
-        <v/>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="str">
-        <f>IF(B12="","",MAX(A$1:A11)+1)</f>
-        <v/>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="str">
-        <f>IF(B13="","",MAX(A$1:A12)+1)</f>
-        <v/>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
+    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E06EC7-760D-4AB5-A9B4-586D9EFD1022}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
-    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="102.77734375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.21875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="18"/>
+    <col min="1" max="1" width="52.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
-        <f>IF(B2="","",MAX(A$1:A1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
-        <f>IF(B3="","",MAX(A$1:A2)+1)</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
-        <f>IF(B4="","",MAX(A$1:A3)+1)</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
-        <f>IF(B5="","",MAX(A$1:A4)+1)</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
-        <f>IF(B6="","",MAX(A$1:A5)+1)</f>
-        <v>5</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <f>IF(B7="","",MAX(A$1:A6)+1)</f>
-        <v>6</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
-        <f>IF(B8="","",MAX(A$1:A7)+1)</f>
-        <v>7</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
-        <f>IF(B9="","",MAX(A$1:A8)+1)</f>
-        <v>8</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="19"/>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
-        <f>IF(B10="","",MAX(A$1:A9)+1)</f>
-        <v>9</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
-        <f>IF(B11="","",MAX(A$1:A10)+1)</f>
-        <v>10</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="str">
-        <f>IF(B12="","",MAX(A$1:A11)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="str">
-        <f>IF(B13="","",MAX(A$1:A12)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="str">
-        <f>IF(B14="","",MAX(A$1:A13)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="str">
-        <f>IF(B15="","",MAX(A$1:A14)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="str">
-        <f>IF(B16="","",MAX(A$1:A15)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="str">
-        <f>IF(B17="","",MAX(A$1:A16)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="str">
-        <f>IF(B18="","",MAX(A$1:A17)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="str">
-        <f>IF(B19="","",MAX(A$1:A18)+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19"/>
-    </row>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add a new User Story, for a new planning
</commit_message>
<xml_diff>
--- a/planning/User Story Version 2017 Start.xlsx
+++ b/planning/User Story Version 2017 Start.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DD35D8E1-3915-454D-9687-7D6A7352AE2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3DCFEF39-7160-4F42-B4B9-CECF58EDB7D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="14244" windowHeight="6996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="17124" windowHeight="6300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funktionen" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="Funktionen">Funktionen!$1:$1048576</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
-  <oleSize ref="A3:H19"/>
+  <oleSize ref="A3:I16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1012,33 +1012,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1063,6 +1036,33 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,8 +1350,8 @@
   </sheetPr>
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,18 +1373,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="61"/>
       <c r="C1" s="24"/>
       <c r="D1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="46" t="s">
         <v>114</v>
       </c>
       <c r="G1" s="25" t="s">
@@ -1407,10 +1407,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="52"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="28">
         <v>1</v>
       </c>
@@ -1524,10 +1524,10 @@
       <c r="L5" s="33"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="50"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="28">
         <f>MAX(C$2:C5)+1</f>
         <v>5</v>
@@ -1582,10 +1582,10 @@
       <c r="L7" s="33"/>
     </row>
     <row r="8" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="28">
         <f>MAX(C$2:C7)+1</f>
         <v>7</v>
@@ -1612,8 +1612,8 @@
       <c r="L8" s="33"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="28"/>
       <c r="D9" s="29">
         <f>IF(G9="","",MAX(D$1:D8)+1)</f>
@@ -1681,11 +1681,11 @@
       <c r="L11" s="33"/>
     </row>
     <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.4">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="29">
         <f>IF(G12="","",MAX(D$1:D11)+1)</f>
         <v>11</v>
@@ -1706,13 +1706,13 @@
       <c r="L12" s="33"/>
     </row>
     <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="59"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="29">
         <f>IF(G13="","",MAX(D$1:D12)+1)</f>
         <v>12</v>
@@ -1735,13 +1735,13 @@
       <c r="L13" s="33"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="59"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="29">
         <f>IF(G14="","",MAX(D$1:D13)+1)</f>
         <v>13</v>
@@ -1764,13 +1764,13 @@
       <c r="L14" s="33"/>
     </row>
     <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="59"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="29">
         <f>IF(G15="","",MAX(D$1:D14)+1)</f>
         <v>14</v>
@@ -1791,13 +1791,13 @@
       <c r="L15" s="33"/>
     </row>
     <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="59"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="29">
         <f>IF(G16="","",MAX(D$1:D15)+1)</f>
         <v>15</v>
@@ -1820,13 +1820,13 @@
       <c r="L16" s="33"/>
     </row>
     <row r="17" spans="1:14" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="59"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="29">
         <f>IF(G17="","",MAX(D$1:D16)+1)</f>
         <v>16</v>
@@ -1846,13 +1846,13 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="29">
         <f>IF(G18="","",MAX(D$1:D17)+1)</f>
         <v>17</v>
@@ -2048,13 +2048,13 @@
       <c r="F30" s="33"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
-      <c r="B34" s="46"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
       <c r="C34" s="44"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" s="46"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="59"/>
       <c r="C35" s="44"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -2732,21 +2732,21 @@
       <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="58" t="s">
         <v>131</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="58" t="s">
         <v>132</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="58" t="s">
         <v>135</v>
       </c>
       <c r="B16" s="12"/>

</xml_diff>